<commit_message>
add key ngoai ht
</commit_message>
<xml_diff>
--- a/src/test/java/seatech/uiTest/pvcb/testcase/PVCB.xlsx
+++ b/src/test/java/seatech/uiTest/pvcb/testcase/PVCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\PVCB_Auto\src\test\java\seatech\uiTest\pvcb\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DA953E-550E-438C-893E-81014F71398C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68CE15A-AA8F-40DB-BDD8-D06B1A83F236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="397">
   <si>
     <t>action</t>
   </si>
@@ -1230,6 +1230,15 @@
   </si>
   <si>
     <t>clickButtonEndTran_interBank</t>
+  </si>
+  <si>
+    <t>10301816_dmaker1</t>
+  </si>
+  <si>
+    <t>activeOTPLater</t>
+  </si>
+  <si>
+    <t>008223361111</t>
   </si>
 </sst>
 </file>
@@ -2041,7 +2050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54311AB6-075D-47AA-B061-AE4D340A8B3C}">
   <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -14725,10 +14734,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32113C54-5D0B-4965-9152-B8DD35EA4C21}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14770,8 +14779,8 @@
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>48</v>
+      <c r="C3" s="54" t="s">
+        <v>394</v>
       </c>
       <c r="D3" s="106"/>
     </row>
@@ -14793,101 +14802,109 @@
       <c r="C5" s="6"/>
       <c r="D5" s="106"/>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>287</v>
+        <v>396</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>384</v>
+        <v>287</v>
       </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>288</v>
+        <v>386</v>
       </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>17</v>
+        <v>288</v>
       </c>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>388</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>17</v>
+      </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
       <c r="B15" s="6" t="s">
-        <v>391</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>393</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add key ngoai ht, verify
</commit_message>
<xml_diff>
--- a/src/test/java/seatech/uiTest/pvcb/testcase/PVCB.xlsx
+++ b/src/test/java/seatech/uiTest/pvcb/testcase/PVCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\PVCB_Auto\src\test\java\seatech\uiTest\pvcb\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68CE15A-AA8F-40DB-BDD8-D06B1A83F236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F069B9C-D688-4B06-B37F-E7F90B89A938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="390">
   <si>
     <t>action</t>
   </si>
@@ -1196,21 +1196,6 @@
     <t>Giao dịch, Chuyển khoản, Chuyển Khoản Ngoài Hệ Thống</t>
   </si>
   <si>
-    <t>enterReceiveAccount_interBank</t>
-  </si>
-  <si>
-    <t>enterReceiveName_interBank</t>
-  </si>
-  <si>
-    <t>VY DOAN</t>
-  </si>
-  <si>
-    <t>selectBankNo_interBank</t>
-  </si>
-  <si>
-    <t>Sacombank - NH TMCP Sai Gon Thuong Tin</t>
-  </si>
-  <si>
     <t>tickAgreeCondition_interBank</t>
   </si>
   <si>
@@ -1232,13 +1217,7 @@
     <t>clickButtonEndTran_interBank</t>
   </si>
   <si>
-    <t>10301816_dmaker1</t>
-  </si>
-  <si>
-    <t>activeOTPLater</t>
-  </si>
-  <si>
-    <t>008223361111</t>
+    <t>chooseSaveReceiveAccount_interBank</t>
   </si>
 </sst>
 </file>
@@ -8734,7 +8713,7 @@
   <dimension ref="A1:D388"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14734,10 +14713,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32113C54-5D0B-4965-9152-B8DD35EA4C21}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14780,7 +14759,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>394</v>
+        <v>48</v>
       </c>
       <c r="D3" s="106"/>
     </row>
@@ -14802,43 +14781,45 @@
       <c r="C5" s="6"/>
       <c r="D5" s="106"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>374</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>396</v>
+        <v>46</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -14848,64 +14829,34 @@
         <v>383</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>384</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>386</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>288</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>